<commit_message>
Working on Timeline 1-2
</commit_message>
<xml_diff>
--- a/src/Cyberpunk2078/Assets/Xlsx/Dialogues.xlsx
+++ b/src/Cyberpunk2078/Assets/Xlsx/Dialogues.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB326D4-99D2-473B-8571-409CCA30A4AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F5737F-8949-48AD-B563-763AD9E4A505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -129,13 +129,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>1-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>N</t>
@@ -190,22 +183,34 @@
     <t>I know you got so many questions. But now, it is not the right time.</t>
   </si>
   <si>
-    <t>Take this. You’ll need it, Mr.Leo.</t>
-  </si>
-  <si>
     <t>Yes...Those AI are looking for me. It’s strange…</t>
   </si>
   <si>
     <t>No matter what, I will be forced to log out if I am caught.</t>
   </si>
   <si>
-    <t>I must get out.</t>
-  </si>
-  <si>
     <t xml:space="preserve">I can’t let them know I’m here. We have to leave here. </t>
   </si>
   <si>
-    <t>Hey! What are you…</t>
+    <t>This is the ‘Key’, the key to touch the world.</t>
+  </si>
+  <si>
+    <t>They are getting here.</t>
+  </si>
+  <si>
+    <t>I will await you in the alley at midnight.</t>
+  </si>
+  <si>
+    <t>I will go out and distract them. Just go.</t>
+  </si>
+  <si>
+    <t>I must get out{action:end}.</t>
+  </si>
+  <si>
+    <t>Hey! What are you...</t>
+  </si>
+  <si>
+    <t>Take this. You’ll need it, Mr.Leo{action:continue}.</t>
   </si>
 </sst>
 </file>
@@ -645,17 +650,17 @@
   <dimension ref="A1:J167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="13"/>
-    <col min="9" max="9" width="9.140625" style="14"/>
-    <col min="10" max="10" width="9.140625" style="13"/>
+    <col min="6" max="6" width="9.1796875" style="13"/>
+    <col min="9" max="9" width="9.1796875" style="14"/>
+    <col min="10" max="10" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="30" customHeight="1">
@@ -690,52 +695,52 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13.9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -743,12 +748,12 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="13.9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -756,12 +761,12 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="13.9">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -769,12 +774,12 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="13.9">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -782,12 +787,12 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="13.9">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -795,12 +800,12 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="13.9">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -808,12 +813,12 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="13.9">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -821,12 +826,12 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="13.9">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -834,12 +839,12 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="13.9">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -847,12 +852,12 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="13.9">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -860,12 +865,12 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="13.9">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -873,12 +878,12 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="13.9">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -886,12 +891,12 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="13.9">
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -899,12 +904,12 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="13.9">
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -912,12 +917,12 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="13.9">
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -925,12 +930,12 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="13.9">
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -938,12 +943,12 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="13.9">
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -951,12 +956,12 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="13.9">
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -964,12 +969,12 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="13.9">
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -977,12 +982,12 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="13.9">
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -990,12 +995,12 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="13.9">
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1003,12 +1008,12 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="13.9">
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1016,12 +1021,12 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="13.9">
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1029,12 +1034,12 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8" ht="13.9">
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1042,12 +1047,12 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8" ht="13.9">
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -1055,12 +1060,12 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" ht="13.9">
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1068,52 +1073,52 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8" ht="13.9">
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="13.9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -1121,12 +1126,12 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="13.9">
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1139,7 +1144,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1147,7 +1152,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1155,7 +1160,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1163,7 +1168,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1171,7 +1176,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1179,7 +1184,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1187,7 +1192,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1195,7 +1200,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1203,7 +1208,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1211,7 +1216,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1219,7 +1224,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1227,7 +1232,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1235,7 +1240,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1243,7 +1248,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1251,7 +1256,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1259,7 +1264,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1267,7 +1272,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1275,7 +1280,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1283,7 +1288,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1291,7 +1296,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1299,7 +1304,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1307,7 +1312,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1315,7 +1320,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1323,7 +1328,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1331,7 +1336,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1339,7 +1344,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1347,7 +1352,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1355,7 +1360,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1363,7 +1368,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1371,7 +1376,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1379,7 +1384,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1387,7 +1392,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1395,7 +1400,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1403,7 +1408,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1411,7 +1416,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1419,7 +1424,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1427,7 +1432,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1435,7 +1440,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1443,7 +1448,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1451,7 +1456,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1459,7 +1464,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1467,7 +1472,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1475,7 +1480,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1483,7 +1488,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1491,7 +1496,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1499,7 +1504,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1507,7 +1512,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1515,7 +1520,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1523,7 +1528,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1531,7 +1536,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1539,7 +1544,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1547,7 +1552,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1555,7 +1560,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1563,7 +1568,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1571,7 +1576,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1579,7 +1584,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1587,7 +1592,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -1595,7 +1600,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -1603,7 +1608,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -1611,7 +1616,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -1619,7 +1624,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -1627,7 +1632,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -1635,16 +1640,16 @@
         <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F102" s="13">
         <v>101</v>
@@ -1658,8 +1663,8 @@
       <c r="I102" s="14">
         <v>1</v>
       </c>
-      <c r="J102" s="13" t="s">
-        <v>36</v>
+      <c r="J102" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -1667,16 +1672,16 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F103" s="13">
         <v>102</v>
@@ -1690,8 +1695,8 @@
       <c r="I103" s="14">
         <v>1</v>
       </c>
-      <c r="J103" s="13" t="s">
-        <v>36</v>
+      <c r="J103" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -1699,16 +1704,16 @@
         <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F104" s="13">
         <v>103</v>
@@ -1722,8 +1727,8 @@
       <c r="I104" s="14">
         <v>1</v>
       </c>
-      <c r="J104" s="13" t="s">
-        <v>37</v>
+      <c r="J104" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -1731,16 +1736,16 @@
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F105" s="13">
         <v>104</v>
@@ -1754,8 +1759,8 @@
       <c r="I105" s="14">
         <v>1</v>
       </c>
-      <c r="J105" s="13" t="s">
-        <v>36</v>
+      <c r="J105" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -1763,16 +1768,16 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F106" s="13">
         <v>105</v>
@@ -1786,8 +1791,8 @@
       <c r="I106" s="14">
         <v>1</v>
       </c>
-      <c r="J106" s="13" t="s">
-        <v>36</v>
+      <c r="J106" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -1795,16 +1800,16 @@
         <v>105</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E107" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F107" s="13">
         <v>106</v>
@@ -1812,8 +1817,8 @@
       <c r="I107" s="14">
         <v>1</v>
       </c>
-      <c r="J107" s="13" t="s">
-        <v>36</v>
+      <c r="J107" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -1821,16 +1826,16 @@
         <v>106</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E108" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F108" s="13">
         <v>107</v>
@@ -1838,8 +1843,8 @@
       <c r="I108" s="14">
         <v>1</v>
       </c>
-      <c r="J108" s="13" t="s">
-        <v>36</v>
+      <c r="J108" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -1847,16 +1852,16 @@
         <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F109" s="13">
         <v>108</v>
@@ -1864,8 +1869,8 @@
       <c r="I109" s="14">
         <v>1</v>
       </c>
-      <c r="J109" s="13" t="s">
-        <v>36</v>
+      <c r="J109" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -1873,16 +1878,16 @@
         <v>108</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E110" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F110" s="13">
         <v>109</v>
@@ -1890,8 +1895,8 @@
       <c r="I110" s="14">
         <v>1</v>
       </c>
-      <c r="J110" s="13" t="s">
-        <v>36</v>
+      <c r="J110" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -1899,16 +1904,16 @@
         <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E111" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F111" s="13">
         <v>110</v>
@@ -1916,8 +1921,8 @@
       <c r="I111" s="14">
         <v>1</v>
       </c>
-      <c r="J111" s="13" t="s">
-        <v>36</v>
+      <c r="J111" s="13">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -1925,16 +1930,16 @@
         <v>110</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E112" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F112" s="13">
         <v>111</v>
@@ -1942,25 +1947,25 @@
       <c r="I112" s="14">
         <v>1</v>
       </c>
-      <c r="J112" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9">
+      <c r="J112" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E113" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F113" s="13">
         <v>112</v>
@@ -1968,22 +1973,25 @@
       <c r="I113" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:9">
+      <c r="J113" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E114" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F114" s="13">
         <v>113</v>
@@ -1991,22 +1999,25 @@
       <c r="I114" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E115" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F115" s="13">
         <v>114</v>
@@ -2014,109 +2025,112 @@
       <c r="I115" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:9">
+      <c r="J115" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>126</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -2124,7 +2138,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -2132,7 +2146,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -2140,7 +2154,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -2148,16 +2162,16 @@
         <v>130</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C132" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D132" t="s">
         <v>35</v>
       </c>
       <c r="E132" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F132" s="13">
         <v>131</v>
@@ -2174,16 +2188,16 @@
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E133" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F133" s="13">
         <v>132</v>
@@ -2200,16 +2214,16 @@
         <v>132</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E134" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F134" s="13">
         <v>133</v>
@@ -2226,16 +2240,19 @@
         <v>133</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="E135" t="s">
+        <v>56</v>
+      </c>
       <c r="F135" s="13">
-        <v>134</v>
+        <v>-1</v>
       </c>
       <c r="I135" s="14">
         <v>1</v>
@@ -2249,13 +2266,16 @@
         <v>134</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="F136" s="13">
         <v>135</v>
@@ -2272,10 +2292,19 @@
         <v>135</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E137" t="s">
+        <v>59</v>
       </c>
       <c r="F137" s="13">
         <v>136</v>
+      </c>
+      <c r="I137" s="14">
+        <v>1</v>
       </c>
       <c r="J137" s="13">
         <v>2</v>
@@ -2286,10 +2315,19 @@
         <v>136</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E138" t="s">
+        <v>58</v>
       </c>
       <c r="F138" s="13">
         <v>137</v>
+      </c>
+      <c r="I138" s="14">
+        <v>1</v>
       </c>
       <c r="J138" s="13">
         <v>2</v>
@@ -2300,10 +2338,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J139" s="13">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -2311,10 +2346,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J140" s="13">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="141" spans="1:10">
@@ -2322,10 +2354,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J141" s="13">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -2333,7 +2362,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -2341,7 +2370,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -2349,7 +2378,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -2357,7 +2386,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -2365,7 +2394,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -2373,7 +2402,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -2381,7 +2410,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -2389,7 +2418,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -2397,7 +2426,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -2405,7 +2434,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -2413,16 +2442,16 @@
         <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C152" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D152" t="s">
         <v>35</v>
       </c>
       <c r="E152" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F152" s="13">
         <v>151</v>
@@ -2431,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="J152" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -2439,13 +2468,13 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C153" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E153" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F153" s="13">
         <v>152</v>
@@ -2454,7 +2483,7 @@
         <v>1</v>
       </c>
       <c r="J153" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -2462,13 +2491,13 @@
         <v>152</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C154" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E154" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F154" s="13">
         <v>-1</v>
@@ -2477,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="J154" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -2485,7 +2514,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -2493,7 +2522,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -2501,7 +2530,10 @@
         <v>155</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C157" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -2509,7 +2541,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -2517,7 +2549,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -2525,7 +2557,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2533,7 +2565,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2541,7 +2573,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2549,7 +2581,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2557,7 +2589,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2565,7 +2597,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2573,7 +2605,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2581,7 +2613,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2602,11 +2634,11 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">

</xml_diff>